<commit_message>
Almost finished, missing the integrator
</commit_message>
<xml_diff>
--- a/EJ4/Derivador/Mediciones/Mediciones Derivador Compensado.xlsx
+++ b/EJ4/Derivador/Mediciones/Mediciones Derivador Compensado.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Indice" sheetId="1" r:id="rId1"/>
@@ -1065,6 +1065,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1204,37 +1205,37 @@
                   <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>200000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>500000</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
                   <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>150000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>300000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1276,37 +1277,37 @@
                   <c:v>16.577822829265173</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>19.852497376387106</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>22.385528152243289</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>22.36350276528929</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>30.539202833168389</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>38.72411994447986</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>42.179598655505728</c:v>
-                </c:pt>
                 <c:pt idx="14">
+                  <c:v>38.214703573636889</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40.56821713825957</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40.947190668604847</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40.300714096456588</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>34.363066414167164</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>28.567283700377708</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
                   <c:v>18.031016873698441</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>22.36350276528929</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19.852497376387106</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>45.432251482907205</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43.337350433529508</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>34.363066414167164</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0</c:v>
@@ -1601,6 +1602,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1751,37 +1753,37 @@
                   <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>200000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>500000</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
                   <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>150000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>180000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>300000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1823,37 +1825,37 @@
                   <c:v>-90</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>-97</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>-96</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>-116</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>-150</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
+                  <c:v>-180</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-229</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>-242</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
+                  <c:v>-278</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>-293</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
                   <c:v>-324</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-96</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-180</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-229</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2318,7 +2320,7 @@
                   <c:v>1709.8445595854923</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1678.695652173913</c:v>
+                  <c:v>1072.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>434.0322580645161</c:v>
@@ -2327,7 +2329,7 @@
                   <c:v>183.3774834437086</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>147.23076923076923</c:v>
+                  <c:v>95.699999999999989</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>41.555555555555564</c:v>
@@ -2754,7 +2756,7 @@
                   <c:v>-90</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80</c:v>
+                  <c:v>-90</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-90</c:v>
@@ -2769,7 +2771,7 @@
                   <c:v>-90</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-80</c:v>
+                  <c:v>-90</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-90</c:v>
@@ -2778,7 +2780,7 @@
                   <c:v>-90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-100</c:v>
+                  <c:v>-90</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>-90</c:v>
@@ -5986,8 +5988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6046,11 +6048,11 @@
         <v>-100</v>
       </c>
       <c r="E3" s="11">
-        <f t="shared" ref="E3:E18" si="0">IF(ISBLANK(C3), , C3/A3)</f>
+        <f t="shared" ref="E3:E23" si="0">IF(ISBLANK(C3), , C3/A3)</f>
         <v>6.3316582914572867E-3</v>
       </c>
       <c r="F3" s="26">
-        <f>IF(E3 = 0, , 20*LOG10(E3))</f>
+        <f t="shared" ref="F3:F23" si="1">IF(E3 = 0, , 20*LOG10(E3))</f>
         <v>-43.969650625842874</v>
       </c>
     </row>
@@ -6072,7 +6074,7 @@
         <v>1.3969849246231158E-2</v>
       </c>
       <c r="F4" s="26">
-        <f t="shared" ref="F4:F40" si="1">IF(E4 = 0, , 20*LOG10(E4))</f>
+        <f t="shared" si="1"/>
         <v>-37.09616560983261</v>
       </c>
     </row>
@@ -6254,248 +6256,248 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
-        <v>1.93</v>
+        <v>2.91</v>
       </c>
       <c r="B13" s="11">
-        <v>20000</v>
+        <v>15000</v>
       </c>
       <c r="C13" s="25">
-        <v>25.4</v>
+        <v>28.61</v>
       </c>
       <c r="D13" s="26">
-        <v>-97</v>
+        <v>-90</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
-        <v>13.160621761658032</v>
+        <v>9.8316151202749129</v>
       </c>
       <c r="F13" s="26">
         <f t="shared" si="1"/>
-        <v>22.385528152243289</v>
+        <v>19.852497376387106</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
-        <v>0.69899999999999995</v>
+        <v>1.93</v>
       </c>
       <c r="B14" s="11">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C14" s="25">
-        <v>23.52</v>
+        <v>25.4</v>
       </c>
       <c r="D14" s="26">
-        <v>-116</v>
+        <v>-97</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
-        <v>33.648068669527902</v>
+        <v>13.160621761658032</v>
       </c>
       <c r="F14" s="26">
         <f t="shared" si="1"/>
-        <v>30.539202833168389</v>
+        <v>22.385528152243289</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
-        <v>0.183</v>
+        <v>1.909</v>
       </c>
       <c r="B15" s="11">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="C15" s="25">
-        <v>15.8</v>
+        <v>25.06</v>
       </c>
       <c r="D15" s="26">
-        <v>-150</v>
+        <v>-96</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
-        <v>86.338797814207652</v>
+        <v>13.127291775798847</v>
       </c>
       <c r="F15" s="26">
         <f t="shared" si="1"/>
-        <v>38.72411994447986</v>
+        <v>22.36350276528929</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="B16" s="11">
+        <v>50000</v>
+      </c>
+      <c r="C16" s="25">
+        <v>23.52</v>
+      </c>
+      <c r="D16" s="26">
+        <v>-116</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="0"/>
+        <v>33.648068669527902</v>
+      </c>
+      <c r="F16" s="26">
+        <f t="shared" si="1"/>
+        <v>30.539202833168389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <v>0.183</v>
+      </c>
+      <c r="B17" s="11">
+        <v>100000</v>
+      </c>
+      <c r="C17" s="25">
+        <v>14.9</v>
+      </c>
+      <c r="D17" s="26">
+        <v>-150</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="0"/>
+        <v>81.420765027322403</v>
+      </c>
+      <c r="F17" s="26">
+        <f t="shared" si="1"/>
+        <v>38.214703573636889</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="B18" s="11">
+        <v>150000</v>
+      </c>
+      <c r="C18" s="25">
+        <v>7.58</v>
+      </c>
+      <c r="D18" s="26">
+        <v>-180</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="0"/>
+        <v>106.7605633802817</v>
+      </c>
+      <c r="F18" s="26">
+        <f t="shared" si="1"/>
+        <v>40.56821713825957</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="B19" s="11">
+        <v>180000</v>
+      </c>
+      <c r="C19" s="25">
+        <v>10.26</v>
+      </c>
+      <c r="D19" s="26">
+        <f>-360+131</f>
+        <v>-229</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="0"/>
+        <v>111.52173913043478</v>
+      </c>
+      <c r="F19" s="26">
+        <f t="shared" si="1"/>
+        <v>40.947190668604847</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B20" s="11">
         <v>200000</v>
       </c>
-      <c r="C16" s="25">
-        <v>11.31</v>
-      </c>
-      <c r="D16" s="26">
+      <c r="C20" s="25">
+        <v>9.11</v>
+      </c>
+      <c r="D20" s="26">
         <f>-360+118</f>
         <v>-242</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E20" s="11">
         <f t="shared" si="0"/>
-        <v>128.52272727272728</v>
-      </c>
-      <c r="F16" s="26">
+        <v>103.52272727272727</v>
+      </c>
+      <c r="F20" s="26">
         <f t="shared" si="1"/>
-        <v>42.179598655505728</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="25">
+        <v>40.300714096456588</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <v>0.155</v>
+      </c>
+      <c r="B21" s="11">
+        <v>300000</v>
+      </c>
+      <c r="C21" s="25">
+        <v>8.1</v>
+      </c>
+      <c r="D21" s="26">
+        <f>82-360</f>
+        <v>-278</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="0"/>
+        <v>52.258064516129032</v>
+      </c>
+      <c r="F21" s="26">
+        <f t="shared" si="1"/>
+        <v>34.363066414167164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
         <v>0.113</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B22" s="11">
         <v>500000</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C22" s="25">
         <v>3.03</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D22" s="26">
         <f>67-360</f>
         <v>-293</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E22" s="11">
         <f t="shared" si="0"/>
         <v>26.814159292035395</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F22" s="26">
         <f t="shared" si="1"/>
         <v>28.567283700377708</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
         <v>0.21199999999999999</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B23" s="11">
         <v>1000000</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C23" s="25">
         <v>1.69</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D23" s="26">
         <v>-324</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E23" s="11">
         <f t="shared" si="0"/>
         <v>7.9716981132075473</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F23" s="26">
         <f t="shared" si="1"/>
         <v>18.031016873698441</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="25">
-        <v>1.909</v>
-      </c>
-      <c r="B19" s="11">
-        <v>20000</v>
-      </c>
-      <c r="C19" s="25">
-        <v>25.06</v>
-      </c>
-      <c r="D19" s="26">
-        <v>-96</v>
-      </c>
-      <c r="E19" s="11">
-        <f t="shared" ref="E19:E21" si="2">IF(ISBLANK(C19), , C19/A19)</f>
-        <v>13.127291775798847</v>
-      </c>
-      <c r="F19" s="26">
-        <f t="shared" si="1"/>
-        <v>22.36350276528929</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="25">
-        <v>2.91</v>
-      </c>
-      <c r="B20" s="11">
-        <v>15000</v>
-      </c>
-      <c r="C20" s="25">
-        <v>28.61</v>
-      </c>
-      <c r="D20" s="26">
-        <v>-90</v>
-      </c>
-      <c r="E20" s="11">
-        <f t="shared" si="2"/>
-        <v>9.8316151202749129</v>
-      </c>
-      <c r="F20" s="26">
-        <f t="shared" si="1"/>
-        <v>19.852497376387106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="25">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="B21" s="11">
-        <v>150000</v>
-      </c>
-      <c r="C21" s="25">
-        <v>13.27</v>
-      </c>
-      <c r="D21" s="26">
-        <v>-180</v>
-      </c>
-      <c r="E21" s="11">
-        <f t="shared" si="2"/>
-        <v>186.90140845070422</v>
-      </c>
-      <c r="F21" s="26">
-        <f t="shared" si="1"/>
-        <v>45.432251482907205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="25">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="B22" s="11">
-        <v>180000</v>
-      </c>
-      <c r="C22" s="25">
-        <v>13.51</v>
-      </c>
-      <c r="D22" s="26">
-        <f>-360+131</f>
-        <v>-229</v>
-      </c>
-      <c r="E22" s="11">
-        <f t="shared" ref="E22:E29" si="3">IF(ISBLANK(C22), , C22/A22)</f>
-        <v>146.84782608695653</v>
-      </c>
-      <c r="F22" s="26">
-        <f t="shared" si="1"/>
-        <v>43.337350433529508</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="25">
-        <v>0.155</v>
-      </c>
-      <c r="B23" s="11">
-        <v>300000</v>
-      </c>
-      <c r="C23" s="25">
-        <v>8.1</v>
-      </c>
-      <c r="D23" s="26">
-        <f>82-360</f>
-        <v>-278</v>
-      </c>
-      <c r="E23" s="11">
-        <f t="shared" si="3"/>
-        <v>52.258064516129032</v>
-      </c>
-      <c r="F23" s="26">
-        <f t="shared" si="1"/>
-        <v>34.363066414167164</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -6504,11 +6506,11 @@
       <c r="C24" s="25"/>
       <c r="D24" s="26"/>
       <c r="E24" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E24:E29" si="2">IF(ISBLANK(C24), , C24/A24)</f>
         <v>0</v>
       </c>
       <c r="F24" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F24:F40" si="3">IF(E24 = 0, , 20*LOG10(E24))</f>
         <v>0</v>
       </c>
     </row>
@@ -6518,11 +6520,11 @@
       <c r="C25" s="25"/>
       <c r="D25" s="26"/>
       <c r="E25" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="26">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6532,11 +6534,11 @@
       <c r="C26" s="25"/>
       <c r="D26" s="26"/>
       <c r="E26" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="26">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6546,11 +6548,11 @@
       <c r="C27" s="25"/>
       <c r="D27" s="26"/>
       <c r="E27" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="26">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6560,11 +6562,11 @@
       <c r="C28" s="25"/>
       <c r="D28" s="26"/>
       <c r="E28" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="26">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6574,11 +6576,11 @@
       <c r="C29" s="25"/>
       <c r="D29" s="26"/>
       <c r="E29" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="26">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6592,7 +6594,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6606,7 +6608,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6620,7 +6622,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6634,7 +6636,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6648,7 +6650,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6662,7 +6664,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6676,7 +6678,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6690,7 +6692,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6704,7 +6706,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6718,7 +6720,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6732,11 +6734,14 @@
         <v>0</v>
       </c>
       <c r="F40" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:F23">
+    <sortCondition ref="B3:B23"/>
+  </sortState>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -6934,8 +6939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7056,7 +7061,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="36">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H4" s="33">
         <f t="shared" ref="H4:H22" si="0">IF(E4 = 0,,F4/E4)</f>
@@ -7068,7 +7073,7 @@
       </c>
       <c r="J4" s="37">
         <f t="shared" ref="J4:J22" si="2" xml:space="preserve"> D4-G4</f>
-        <v>-80</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -7225,7 +7230,7 @@
         <v>17.3</v>
       </c>
       <c r="G9" s="36">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H9" s="33">
         <f t="shared" si="0"/>
@@ -7237,7 +7242,7 @@
       </c>
       <c r="J9" s="37">
         <f t="shared" si="2"/>
-        <v>-80</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -7323,22 +7328,22 @@
         <v>390</v>
       </c>
       <c r="F12" s="35">
-        <v>0.23</v>
+        <v>0.36</v>
       </c>
       <c r="G12" s="36">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H12" s="33">
         <f t="shared" si="0"/>
-        <v>5.8974358974358979E-4</v>
+        <v>9.2307692307692305E-4</v>
       </c>
       <c r="I12" s="33">
         <f t="shared" si="1"/>
-        <v>1678.695652173913</v>
+        <v>1072.5</v>
       </c>
       <c r="J12" s="37">
         <f t="shared" si="2"/>
-        <v>-100</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -7424,18 +7429,18 @@
         <v>22</v>
       </c>
       <c r="F15" s="35">
-        <v>0.13</v>
+        <v>0.2</v>
       </c>
       <c r="G15" s="36">
         <v>10</v>
       </c>
       <c r="H15" s="33">
         <f t="shared" si="0"/>
-        <v>5.909090909090909E-3</v>
+        <v>9.0909090909090922E-3</v>
       </c>
       <c r="I15" s="33">
         <f t="shared" si="1"/>
-        <v>147.23076923076923</v>
+        <v>95.699999999999989</v>
       </c>
       <c r="J15" s="37">
         <f t="shared" si="2"/>

</xml_diff>